<commit_message>
new datasets + potpourri modification
</commit_message>
<xml_diff>
--- a/mpath/src/data/toronto_all.xlsx
+++ b/mpath/src/data/toronto_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SuhasVittal/Documents/programming/quantum_computing/mpath/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4781F9B5-11F2-9242-B8D7-01A4D870B81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C192880-9D64-9847-8A2B-5223B6770E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="880" windowWidth="18720" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>SABRE CNOTs</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>vqe_uccsd_n6</t>
+  </si>
+  <si>
+    <t>geomean</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T105"/>
+  <dimension ref="A1:T106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="61" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,13 +1387,13 @@
       <c r="R2">
         <v>0</v>
       </c>
-      <c r="S2" t="e" cm="1">
+      <c r="S2" cm="1">
         <f t="array" aca="1" ref="S2" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C2,$G2)), ($C2:$G2),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T2" t="e" cm="1">
+        <v>144</v>
+      </c>
+      <c r="T2" cm="1">
         <f t="array" aca="1" ref="T2" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C2,$G2)), ($C2:$G2),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1448,13 +1451,13 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="S3" t="e" cm="1">
+      <c r="S3" cm="1">
         <f t="array" aca="1" ref="S3" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C3,$G3)), ($C3:$G3),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T3" t="e" cm="1">
+        <v>183</v>
+      </c>
+      <c r="T3" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C3,$G3)), ($C3:$G3),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1512,13 +1515,13 @@
       <c r="R4">
         <v>0</v>
       </c>
-      <c r="S4" t="e" cm="1">
+      <c r="S4" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C4,$G4)), ($C4:$G4),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T4" t="e" cm="1">
+        <v>867</v>
+      </c>
+      <c r="T4" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C4,$G4)), ($C4:$G4),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -1576,13 +1579,13 @@
       <c r="R5">
         <v>0</v>
       </c>
-      <c r="S5" t="e" cm="1">
+      <c r="S5" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C5,$G5)), ($C5:$G5),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T5" t="e" cm="1">
+        <v>333</v>
+      </c>
+      <c r="T5" cm="1">
         <f t="array" aca="1" ref="T5" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C5,$G5)), ($C5:$G5),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>625</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -1640,13 +1643,13 @@
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="S6" t="e" cm="1">
+      <c r="S6" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C6,$G6)), ($C6:$G6),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T6" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="T6" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C6,$G6)), ($C6:$G6),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -1704,13 +1707,13 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7" t="e" cm="1">
+      <c r="S7" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C7,$G7)), ($C7:$G7),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T7" t="e" cm="1">
+        <v>3039</v>
+      </c>
+      <c r="T7" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C7,$G7)), ($C7:$G7),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>4810</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -1768,13 +1771,13 @@
       <c r="R8">
         <v>0</v>
       </c>
-      <c r="S8" t="e" cm="1">
+      <c r="S8" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C8,$G8)), ($C8:$G8),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T8" t="e" cm="1">
+        <v>126</v>
+      </c>
+      <c r="T8" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C8,$G8)), ($C8:$G8),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -1832,13 +1835,13 @@
       <c r="R9">
         <v>0</v>
       </c>
-      <c r="S9" t="e" cm="1">
+      <c r="S9" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C9,$G9)), ($C9:$G9),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T9" t="e" cm="1">
+        <v>378</v>
+      </c>
+      <c r="T9" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C9,$G9)), ($C9:$G9),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>674</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -1896,13 +1899,13 @@
       <c r="R10">
         <v>0</v>
       </c>
-      <c r="S10" t="e" cm="1">
+      <c r="S10" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C10,$G10)), ($C10:$G10),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T10" t="e" cm="1">
+        <v>201</v>
+      </c>
+      <c r="T10" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C10,$G10)), ($C10:$G10),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1960,13 +1963,13 @@
       <c r="R11">
         <v>0</v>
       </c>
-      <c r="S11" t="e" cm="1">
+      <c r="S11" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C11,$G11)), ($C11:$G11),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T11" t="e" cm="1">
+        <v>861</v>
+      </c>
+      <c r="T11" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C11,$G11)), ($C11:$G11),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -2024,13 +2027,13 @@
       <c r="R12">
         <v>0</v>
       </c>
-      <c r="S12" t="e" cm="1">
+      <c r="S12" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C12,$G12)), ($C12:$G12),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T12" t="e" cm="1">
+        <v>258</v>
+      </c>
+      <c r="T12" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C12,$G12)), ($C12:$G12),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -2088,13 +2091,13 @@
       <c r="R13">
         <v>0</v>
       </c>
-      <c r="S13" t="e" cm="1">
+      <c r="S13" cm="1">
         <f t="array" aca="1" ref="S13" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C13,$G13)), ($C13:$G13),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T13" t="e" cm="1">
+        <v>57</v>
+      </c>
+      <c r="T13" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C13,$G13)), ($C13:$G13),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -2152,13 +2155,13 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14" t="e" cm="1">
+      <c r="S14" cm="1">
         <f t="array" aca="1" ref="S14" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C14,$G14)), ($C14:$G14),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T14" t="e" cm="1">
+        <v>99</v>
+      </c>
+      <c r="T14" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C14,$G14)), ($C14:$G14),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -2216,13 +2219,13 @@
       <c r="R15">
         <v>0</v>
       </c>
-      <c r="S15" t="e" cm="1">
+      <c r="S15" cm="1">
         <f t="array" aca="1" ref="S15" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C15,$G15)), ($C15:$G15),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T15" t="e" cm="1">
+        <v>78</v>
+      </c>
+      <c r="T15" cm="1">
         <f t="array" aca="1" ref="T15" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C15,$G15)), ($C15:$G15),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -2280,13 +2283,13 @@
       <c r="R16">
         <v>0</v>
       </c>
-      <c r="S16" t="e" cm="1">
+      <c r="S16" cm="1">
         <f t="array" aca="1" ref="S16" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C16,$G16)), ($C16:$G16),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T16" t="e" cm="1">
+        <v>315</v>
+      </c>
+      <c r="T16" cm="1">
         <f t="array" aca="1" ref="T16" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C16,$G16)), ($C16:$G16),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>566</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -2344,13 +2347,13 @@
       <c r="R17">
         <v>0</v>
       </c>
-      <c r="S17" t="e" cm="1">
+      <c r="S17" cm="1">
         <f t="array" aca="1" ref="S17" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C17,$G17)), ($C17:$G17),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T17" t="e" cm="1">
+        <v>3306</v>
+      </c>
+      <c r="T17" cm="1">
         <f t="array" aca="1" ref="T17" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C17,$G17)), ($C17:$G17),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>5056</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -2408,13 +2411,13 @@
       <c r="R18">
         <v>0</v>
       </c>
-      <c r="S18" t="e" cm="1">
+      <c r="S18" cm="1">
         <f t="array" aca="1" ref="S18" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C18,$G18)), ($C18:$G18),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T18" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="T18" cm="1">
         <f t="array" aca="1" ref="T18" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C18,$G18)), ($C18:$G18),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -2472,13 +2475,13 @@
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19" t="e" cm="1">
+      <c r="S19" cm="1">
         <f t="array" aca="1" ref="S19" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C19,$G19)), ($C19:$G19),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T19" t="e" cm="1">
+        <v>219</v>
+      </c>
+      <c r="T19" cm="1">
         <f t="array" aca="1" ref="T19" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C19,$G19)), ($C19:$G19),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -2536,13 +2539,13 @@
       <c r="R20">
         <v>0</v>
       </c>
-      <c r="S20" t="e" cm="1">
+      <c r="S20" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C20,$G20)), ($C20:$G20),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T20" t="e" cm="1">
+        <v>372</v>
+      </c>
+      <c r="T20" cm="1">
         <f t="array" aca="1" ref="T20" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C20,$G20)), ($C20:$G20),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>677</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -2600,13 +2603,13 @@
       <c r="R21">
         <v>0</v>
       </c>
-      <c r="S21" t="e" cm="1">
+      <c r="S21" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C21,$G21)), ($C21:$G21),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T21" t="e" cm="1">
+        <v>69</v>
+      </c>
+      <c r="T21" cm="1">
         <f t="array" aca="1" ref="T21" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C21,$G21)), ($C21:$G21),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -2664,13 +2667,13 @@
       <c r="R22">
         <v>0</v>
       </c>
-      <c r="S22" t="e" cm="1">
+      <c r="S22" cm="1">
         <f t="array" aca="1" ref="S22" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C22,$G22)), ($C22:$G22),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T22" t="e" cm="1">
+        <v>390</v>
+      </c>
+      <c r="T22" cm="1">
         <f t="array" aca="1" ref="T22" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C22,$G22)), ($C22:$G22),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>668</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -2728,13 +2731,13 @@
       <c r="R23">
         <v>0</v>
       </c>
-      <c r="S23" t="e" cm="1">
+      <c r="S23" cm="1">
         <f t="array" aca="1" ref="S23" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C23,$G23)), ($C23:$G23),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T23" t="e" cm="1">
+        <v>144</v>
+      </c>
+      <c r="T23" cm="1">
         <f t="array" aca="1" ref="T23" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C23,$G23)), ($C23:$G23),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -2792,13 +2795,13 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" t="e" cm="1">
+      <c r="S24" cm="1">
         <f t="array" aca="1" ref="S24" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C24,$G24)), ($C24:$G24),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T24" t="e" cm="1">
+        <v>111</v>
+      </c>
+      <c r="T24" cm="1">
         <f t="array" aca="1" ref="T24" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C24,$G24)), ($C24:$G24),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -2856,13 +2859,13 @@
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" t="e" cm="1">
+      <c r="S25" cm="1">
         <f t="array" aca="1" ref="S25" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C25,$G25)), ($C25:$G25),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T25" t="e" cm="1">
+        <v>2775</v>
+      </c>
+      <c r="T25" cm="1">
         <f t="array" aca="1" ref="T25" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C25,$G25)), ($C25:$G25),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -2920,13 +2923,13 @@
       <c r="R26">
         <v>0</v>
       </c>
-      <c r="S26" t="e" cm="1">
+      <c r="S26" cm="1">
         <f t="array" aca="1" ref="S26" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C26,$G26)), ($C26:$G26),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T26" t="e" cm="1">
+        <v>531</v>
+      </c>
+      <c r="T26" cm="1">
         <f t="array" aca="1" ref="T26" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C26,$G26)), ($C26:$G26),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>873</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -2984,13 +2987,13 @@
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27" t="e" cm="1">
+      <c r="S27" cm="1">
         <f t="array" aca="1" ref="S27" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C27,$G27)), ($C27:$G27),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T27" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="T27" cm="1">
         <f t="array" aca="1" ref="T27" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C27,$G27)), ($C27:$G27),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -3048,13 +3051,13 @@
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28" t="e" cm="1">
+      <c r="S28" cm="1">
         <f t="array" aca="1" ref="S28" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C28,$G28)), ($C28:$G28),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T28" t="e" cm="1">
+        <v>66</v>
+      </c>
+      <c r="T28" cm="1">
         <f t="array" aca="1" ref="T28" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C28,$G28)), ($C28:$G28),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -3112,13 +3115,13 @@
       <c r="R29">
         <v>0</v>
       </c>
-      <c r="S29" t="e" cm="1">
+      <c r="S29" cm="1">
         <f t="array" aca="1" ref="S29" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C29,$G29)), ($C29:$G29),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T29" t="e" cm="1">
+        <v>246</v>
+      </c>
+      <c r="T29" cm="1">
         <f t="array" aca="1" ref="T29" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C29,$G29)), ($C29:$G29),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -3176,13 +3179,13 @@
       <c r="R30">
         <v>0</v>
       </c>
-      <c r="S30" t="e" cm="1">
+      <c r="S30" cm="1">
         <f t="array" aca="1" ref="S30" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C30,$G30)), ($C30:$G30),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T30" t="e" cm="1">
+        <v>48</v>
+      </c>
+      <c r="T30" cm="1">
         <f t="array" aca="1" ref="T30" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C30,$G30)), ($C30:$G30),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -3240,13 +3243,13 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="S31" t="e" cm="1">
+      <c r="S31" cm="1">
         <f t="array" aca="1" ref="S31" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C31,$G31)), ($C31:$G31),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T31" t="e" cm="1">
+        <v>1653</v>
+      </c>
+      <c r="T31" cm="1">
         <f t="array" aca="1" ref="T31" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C31,$G31)), ($C31:$G31),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -3304,13 +3307,13 @@
       <c r="R32">
         <v>0</v>
       </c>
-      <c r="S32" t="e" cm="1">
+      <c r="S32" cm="1">
         <f t="array" aca="1" ref="S32" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C32,$G32)), ($C32:$G32),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T32" t="e" cm="1">
+        <v>255</v>
+      </c>
+      <c r="T32" cm="1">
         <f t="array" aca="1" ref="T32" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C32,$G32)), ($C32:$G32),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>458</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -3368,13 +3371,13 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="S33" t="e" cm="1">
+      <c r="S33" cm="1">
         <f t="array" aca="1" ref="S33" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C33,$G33)), ($C33:$G33),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T33" t="e" cm="1">
+        <v>42</v>
+      </c>
+      <c r="T33" cm="1">
         <f t="array" aca="1" ref="T33" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C33,$G33)), ($C33:$G33),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -3432,13 +3435,13 @@
       <c r="R34">
         <v>0</v>
       </c>
-      <c r="S34" t="e" cm="1">
+      <c r="S34" cm="1">
         <f t="array" aca="1" ref="S34" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C34,$G34)), ($C34:$G34),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T34" t="e" cm="1">
+        <v>432</v>
+      </c>
+      <c r="T34" cm="1">
         <f t="array" aca="1" ref="T34" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C34,$G34)), ($C34:$G34),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>783</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -3496,13 +3499,13 @@
       <c r="R35">
         <v>0</v>
       </c>
-      <c r="S35" t="e" cm="1">
+      <c r="S35" cm="1">
         <f t="array" aca="1" ref="S35" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C35,$G35)), ($C35:$G35),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T35" t="e" cm="1">
+        <v>45</v>
+      </c>
+      <c r="T35" cm="1">
         <f t="array" aca="1" ref="T35" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C35,$G35)), ($C35:$G35),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -3560,13 +3563,13 @@
       <c r="R36">
         <v>0</v>
       </c>
-      <c r="S36" t="e" cm="1">
+      <c r="S36" cm="1">
         <f t="array" aca="1" ref="S36" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C36,$G36)), ($C36:$G36),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T36" t="e" cm="1">
+        <v>354</v>
+      </c>
+      <c r="T36" cm="1">
         <f t="array" aca="1" ref="T36" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C36,$G36)), ($C36:$G36),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>634</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -3624,13 +3627,13 @@
       <c r="R37">
         <v>0</v>
       </c>
-      <c r="S37" t="e" cm="1">
+      <c r="S37" cm="1">
         <f t="array" aca="1" ref="S37" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C37,$G37)), ($C37:$G37),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T37" t="e" cm="1">
+        <v>615</v>
+      </c>
+      <c r="T37" cm="1">
         <f t="array" aca="1" ref="T37" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C37,$G37)), ($C37:$G37),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -3688,13 +3691,13 @@
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="S38" t="e" cm="1">
+      <c r="S38" cm="1">
         <f t="array" aca="1" ref="S38" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C38,$G38)), ($C38:$G38),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T38" t="e" cm="1">
+        <v>1536</v>
+      </c>
+      <c r="T38" cm="1">
         <f t="array" aca="1" ref="T38" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C38,$G38)), ($C38:$G38),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -3752,13 +3755,13 @@
       <c r="R39">
         <v>0</v>
       </c>
-      <c r="S39" t="e" cm="1">
+      <c r="S39" cm="1">
         <f t="array" aca="1" ref="S39" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C39,$G39)), ($C39:$G39),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T39" t="e" cm="1">
+        <v>174</v>
+      </c>
+      <c r="T39" cm="1">
         <f t="array" aca="1" ref="T39" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C39,$G39)), ($C39:$G39),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -3816,13 +3819,13 @@
       <c r="R40">
         <v>0</v>
       </c>
-      <c r="S40" t="e" cm="1">
+      <c r="S40" cm="1">
         <f t="array" aca="1" ref="S40" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C40,$G40)), ($C40:$G40),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T40" t="e" cm="1">
+        <v>1503</v>
+      </c>
+      <c r="T40" cm="1">
         <f t="array" aca="1" ref="T40" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C40,$G40)), ($C40:$G40),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -3880,13 +3883,13 @@
       <c r="R41">
         <v>0</v>
       </c>
-      <c r="S41" t="e" cm="1">
+      <c r="S41" cm="1">
         <f t="array" aca="1" ref="S41" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C41,$G41)), ($C41:$G41),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T41" t="e" cm="1">
+        <v>165</v>
+      </c>
+      <c r="T41" cm="1">
         <f t="array" aca="1" ref="T41" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C41,$G41)), ($C41:$G41),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>322</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -3944,13 +3947,13 @@
       <c r="R42">
         <v>0</v>
       </c>
-      <c r="S42" t="e" cm="1">
+      <c r="S42" cm="1">
         <f t="array" aca="1" ref="S42" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C42,$G42)), ($C42:$G42),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T42" t="e" cm="1">
+        <v>60</v>
+      </c>
+      <c r="T42" cm="1">
         <f t="array" aca="1" ref="T42" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C42,$G42)), ($C42:$G42),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -4008,13 +4011,13 @@
       <c r="R43">
         <v>0</v>
       </c>
-      <c r="S43" t="e" cm="1">
+      <c r="S43" cm="1">
         <f t="array" aca="1" ref="S43" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C43,$G43)), ($C43:$G43),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T43" t="e" cm="1">
+        <v>156</v>
+      </c>
+      <c r="T43" cm="1">
         <f t="array" aca="1" ref="T43" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C43,$G43)), ($C43:$G43),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -4072,13 +4075,13 @@
       <c r="R44">
         <v>0</v>
       </c>
-      <c r="S44" t="e" cm="1">
+      <c r="S44" cm="1">
         <f t="array" aca="1" ref="S44" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C44,$G44)), ($C44:$G44),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T44" t="e" cm="1">
+        <v>108</v>
+      </c>
+      <c r="T44" cm="1">
         <f t="array" aca="1" ref="T44" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C44,$G44)), ($C44:$G44),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -4136,13 +4139,13 @@
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="S45" t="e" cm="1">
+      <c r="S45" cm="1">
         <f t="array" aca="1" ref="S45" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C45,$G45)), ($C45:$G45),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T45" t="e" cm="1">
+        <v>168</v>
+      </c>
+      <c r="T45" cm="1">
         <f t="array" aca="1" ref="T45" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C45,$G45)), ($C45:$G45),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -4200,13 +4203,13 @@
       <c r="R46">
         <v>0</v>
       </c>
-      <c r="S46" t="e" cm="1">
+      <c r="S46" cm="1">
         <f t="array" aca="1" ref="S46" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C46,$G46)), ($C46:$G46),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T46" t="e" cm="1">
+        <v>36</v>
+      </c>
+      <c r="T46" cm="1">
         <f t="array" aca="1" ref="T46" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C46,$G46)), ($C46:$G46),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -4264,13 +4267,13 @@
       <c r="R47">
         <v>0</v>
       </c>
-      <c r="S47" t="e" cm="1">
+      <c r="S47" cm="1">
         <f t="array" aca="1" ref="S47" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C47,$G47)), ($C47:$G47),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T47" t="e" cm="1">
+        <v>102</v>
+      </c>
+      <c r="T47" cm="1">
         <f t="array" aca="1" ref="T47" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C47,$G47)), ($C47:$G47),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -4328,13 +4331,13 @@
       <c r="R48">
         <v>0</v>
       </c>
-      <c r="S48" t="e" cm="1">
+      <c r="S48" cm="1">
         <f t="array" aca="1" ref="S48" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C48,$G48)), ($C48:$G48),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T48" t="e" cm="1">
+        <v>138</v>
+      </c>
+      <c r="T48" cm="1">
         <f t="array" aca="1" ref="T48" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C48,$G48)), ($C48:$G48),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
@@ -4392,13 +4395,13 @@
       <c r="R49">
         <v>0</v>
       </c>
-      <c r="S49" t="e" cm="1">
+      <c r="S49" cm="1">
         <f t="array" aca="1" ref="S49" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C49,$G49)), ($C49:$G49),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T49" t="e" cm="1">
+        <v>273</v>
+      </c>
+      <c r="T49" cm="1">
         <f t="array" aca="1" ref="T49" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C49,$G49)), ($C49:$G49),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>466</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
@@ -4456,13 +4459,13 @@
       <c r="R50">
         <v>0</v>
       </c>
-      <c r="S50" t="e" cm="1">
+      <c r="S50" cm="1">
         <f t="array" aca="1" ref="S50" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C50,$G50)), ($C50:$G50),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T50" t="e" cm="1">
+        <v>147</v>
+      </c>
+      <c r="T50" cm="1">
         <f t="array" aca="1" ref="T50" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C50,$G50)), ($C50:$G50),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
@@ -4520,13 +4523,13 @@
       <c r="R51">
         <v>0</v>
       </c>
-      <c r="S51" t="e" cm="1">
+      <c r="S51" cm="1">
         <f t="array" aca="1" ref="S51" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C51,$G51)), ($C51:$G51),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T51" t="e" cm="1">
+        <v>54</v>
+      </c>
+      <c r="T51" cm="1">
         <f t="array" aca="1" ref="T51" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C51,$G51)), ($C51:$G51),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
@@ -4584,13 +4587,13 @@
       <c r="R52">
         <v>0</v>
       </c>
-      <c r="S52" t="e" cm="1">
+      <c r="S52" cm="1">
         <f t="array" aca="1" ref="S52" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C52,$G52)), ($C52:$G52),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T52" t="e" cm="1">
+        <v>27</v>
+      </c>
+      <c r="T52" cm="1">
         <f t="array" aca="1" ref="T52" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C52,$G52)), ($C52:$G52),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
@@ -4648,13 +4651,13 @@
       <c r="R53">
         <v>0</v>
       </c>
-      <c r="S53" t="e" cm="1">
+      <c r="S53" cm="1">
         <f t="array" aca="1" ref="S53" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C53,$G53)), ($C53:$G53),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T53" t="e" cm="1">
+        <v>207</v>
+      </c>
+      <c r="T53" cm="1">
         <f t="array" aca="1" ref="T53" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C53,$G53)), ($C53:$G53),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -4712,13 +4715,13 @@
       <c r="R54">
         <v>0</v>
       </c>
-      <c r="S54" t="e" cm="1">
+      <c r="S54" cm="1">
         <f t="array" aca="1" ref="S54" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C54,$G54)), ($C54:$G54),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T54" t="e" cm="1">
+        <v>198</v>
+      </c>
+      <c r="T54" cm="1">
         <f t="array" aca="1" ref="T54" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C54,$G54)), ($C54:$G54),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>345</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
@@ -4776,13 +4779,13 @@
       <c r="R55">
         <v>0</v>
       </c>
-      <c r="S55" t="e" cm="1">
+      <c r="S55" cm="1">
         <f t="array" aca="1" ref="S55" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C55,$G55)), ($C55:$G55),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T55" t="e" cm="1">
+        <v>201</v>
+      </c>
+      <c r="T55" cm="1">
         <f t="array" aca="1" ref="T55" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C55,$G55)), ($C55:$G55),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>356</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
@@ -4840,13 +4843,13 @@
       <c r="R56">
         <v>0</v>
       </c>
-      <c r="S56" t="e" cm="1">
+      <c r="S56" cm="1">
         <f t="array" aca="1" ref="S56" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C56,$G56)), ($C56:$G56),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T56" t="e" cm="1">
+        <v>51</v>
+      </c>
+      <c r="T56" cm="1">
         <f t="array" aca="1" ref="T56" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C56,$G56)), ($C56:$G56),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
@@ -4904,13 +4907,13 @@
       <c r="R57">
         <v>0</v>
       </c>
-      <c r="S57" t="e" cm="1">
+      <c r="S57" cm="1">
         <f t="array" aca="1" ref="S57" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C57,$G57)), ($C57:$G57),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T57" t="e" cm="1">
+        <v>609</v>
+      </c>
+      <c r="T57" cm="1">
         <f t="array" aca="1" ref="T57" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C57,$G57)), ($C57:$G57),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -4968,13 +4971,13 @@
       <c r="R58">
         <v>0</v>
       </c>
-      <c r="S58" t="e" cm="1">
+      <c r="S58" cm="1">
         <f t="array" aca="1" ref="S58" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C58,$G58)), ($C58:$G58),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T58" t="e" cm="1">
+        <v>39</v>
+      </c>
+      <c r="T58" cm="1">
         <f t="array" aca="1" ref="T58" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C58,$G58)), ($C58:$G58),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
@@ -5032,13 +5035,13 @@
       <c r="R59">
         <v>0</v>
       </c>
-      <c r="S59" t="e" cm="1">
+      <c r="S59" cm="1">
         <f t="array" aca="1" ref="S59" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C59,$G59)), ($C59:$G59),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T59" t="e" cm="1">
+        <v>480</v>
+      </c>
+      <c r="T59" cm="1">
         <f t="array" aca="1" ref="T59" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C59,$G59)), ($C59:$G59),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>906</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
@@ -5096,13 +5099,13 @@
       <c r="R60">
         <v>0</v>
       </c>
-      <c r="S60" t="e" cm="1">
+      <c r="S60" cm="1">
         <f t="array" aca="1" ref="S60" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C60,$G60)), ($C60:$G60),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T60" t="e" cm="1">
+        <v>1116</v>
+      </c>
+      <c r="T60" cm="1">
         <f t="array" aca="1" ref="T60" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C60,$G60)), ($C60:$G60),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
@@ -5160,13 +5163,13 @@
       <c r="R61">
         <v>0</v>
       </c>
-      <c r="S61" t="e" cm="1">
+      <c r="S61" cm="1">
         <f t="array" aca="1" ref="S61" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C61,$G61)), ($C61:$G61),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T61" t="e" cm="1">
+        <v>243</v>
+      </c>
+      <c r="T61" cm="1">
         <f t="array" aca="1" ref="T61" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C61,$G61)), ($C61:$G61),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
@@ -5224,13 +5227,13 @@
       <c r="R62">
         <v>0</v>
       </c>
-      <c r="S62" t="e" cm="1">
+      <c r="S62" cm="1">
         <f t="array" aca="1" ref="S62" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C62,$G62)), ($C62:$G62),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T62" t="e" cm="1">
+        <v>237</v>
+      </c>
+      <c r="T62" cm="1">
         <f t="array" aca="1" ref="T62" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C62,$G62)), ($C62:$G62),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>422</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -5288,13 +5291,13 @@
       <c r="R63">
         <v>0</v>
       </c>
-      <c r="S63" t="e" cm="1">
+      <c r="S63" cm="1">
         <f t="array" aca="1" ref="S63" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C63,$G63)), ($C63:$G63),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T63" t="e" cm="1">
+        <v>54</v>
+      </c>
+      <c r="T63" cm="1">
         <f t="array" aca="1" ref="T63" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C63,$G63)), ($C63:$G63),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
@@ -5352,13 +5355,13 @@
       <c r="R64">
         <v>0</v>
       </c>
-      <c r="S64" t="e" cm="1">
+      <c r="S64" cm="1">
         <f t="array" aca="1" ref="S64" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C64,$G64)), ($C64:$G64),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T64" t="e" cm="1">
+        <v>990</v>
+      </c>
+      <c r="T64" cm="1">
         <f t="array" aca="1" ref="T64" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C64,$G64)), ($C64:$G64),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
@@ -5416,13 +5419,13 @@
       <c r="R65">
         <v>0</v>
       </c>
-      <c r="S65" t="e" cm="1">
+      <c r="S65" cm="1">
         <f t="array" aca="1" ref="S65" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C65,$G65)), ($C65:$G65),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T65" t="e" cm="1">
+        <v>105</v>
+      </c>
+      <c r="T65" cm="1">
         <f t="array" aca="1" ref="T65" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C65,$G65)), ($C65:$G65),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
@@ -5480,13 +5483,13 @@
       <c r="R66">
         <v>0</v>
       </c>
-      <c r="S66" t="e" cm="1">
+      <c r="S66" cm="1">
         <f t="array" aca="1" ref="S66" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C66,$G66)), ($C66:$G66),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T66" t="e" cm="1">
+        <v>123</v>
+      </c>
+      <c r="T66" cm="1">
         <f t="array" aca="1" ref="T66" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C66,$G66)), ($C66:$G66),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
@@ -5544,13 +5547,13 @@
       <c r="R67">
         <v>0</v>
       </c>
-      <c r="S67" t="e" cm="1">
+      <c r="S67" cm="1">
         <f t="array" aca="1" ref="S67" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C67,$G67)), ($C67:$G67),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T67" t="e" cm="1">
+        <v>1080</v>
+      </c>
+      <c r="T67" cm="1">
         <f t="array" aca="1" ref="T67" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C67,$G67)), ($C67:$G67),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
@@ -5608,13 +5611,13 @@
       <c r="R68">
         <v>0</v>
       </c>
-      <c r="S68" t="e" cm="1">
+      <c r="S68" cm="1">
         <f t="array" aca="1" ref="S68" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C68,$G68)), ($C68:$G68),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T68" t="e" cm="1">
+        <v>1734</v>
+      </c>
+      <c r="T68" cm="1">
         <f t="array" aca="1" ref="T68" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C68,$G68)), ($C68:$G68),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
@@ -5672,13 +5675,13 @@
       <c r="R69">
         <v>0</v>
       </c>
-      <c r="S69" t="e" cm="1">
+      <c r="S69" cm="1">
         <f t="array" aca="1" ref="S69" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C69,$G69)), ($C69:$G69),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T69" t="e" cm="1">
+        <v>174</v>
+      </c>
+      <c r="T69" cm="1">
         <f t="array" aca="1" ref="T69" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C69,$G69)), ($C69:$G69),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>344</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
@@ -5736,13 +5739,13 @@
       <c r="R70">
         <v>0</v>
       </c>
-      <c r="S70" t="e" cm="1">
+      <c r="S70" cm="1">
         <f t="array" aca="1" ref="S70" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C70,$G70)), ($C70:$G70),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T70" t="e" cm="1">
+        <v>42</v>
+      </c>
+      <c r="T70" cm="1">
         <f t="array" aca="1" ref="T70" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C70,$G70)), ($C70:$G70),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -5800,13 +5803,13 @@
       <c r="R71">
         <v>0</v>
       </c>
-      <c r="S71" t="e" cm="1">
+      <c r="S71" cm="1">
         <f t="array" aca="1" ref="S71" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C71,$G71)), ($C71:$G71),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T71" t="e" cm="1">
+        <v>303</v>
+      </c>
+      <c r="T71" cm="1">
         <f t="array" aca="1" ref="T71" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C71,$G71)), ($C71:$G71),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>590</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
@@ -5864,13 +5867,13 @@
       <c r="R72">
         <v>0</v>
       </c>
-      <c r="S72" t="e" cm="1">
+      <c r="S72" cm="1">
         <f t="array" aca="1" ref="S72" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C72,$G72)), ($C72:$G72),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T72" t="e" cm="1">
+        <v>213</v>
+      </c>
+      <c r="T72" cm="1">
         <f t="array" aca="1" ref="T72" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C72,$G72)), ($C72:$G72),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
@@ -5928,13 +5931,13 @@
       <c r="R73">
         <v>0</v>
       </c>
-      <c r="S73" t="e" cm="1">
+      <c r="S73" cm="1">
         <f t="array" aca="1" ref="S73" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C73,$G73)), ($C73:$G73),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T73" t="e" cm="1">
+        <v>312</v>
+      </c>
+      <c r="T73" cm="1">
         <f t="array" aca="1" ref="T73" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C73,$G73)), ($C73:$G73),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>390</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
@@ -5992,13 +5995,13 @@
       <c r="R74">
         <v>0</v>
       </c>
-      <c r="S74" t="e" cm="1">
+      <c r="S74" cm="1">
         <f t="array" aca="1" ref="S74" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C74,$G74)), ($C74:$G74),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T74" t="e" cm="1">
+        <v>114</v>
+      </c>
+      <c r="T74" cm="1">
         <f t="array" aca="1" ref="T74" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C74,$G74)), ($C74:$G74),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
@@ -6056,13 +6059,13 @@
       <c r="R75">
         <v>0</v>
       </c>
-      <c r="S75" t="e" cm="1">
+      <c r="S75" cm="1">
         <f t="array" aca="1" ref="S75" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C75,$G75)), ($C75:$G75),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T75" t="e" cm="1">
+        <v>1005</v>
+      </c>
+      <c r="T75" cm="1">
         <f t="array" aca="1" ref="T75" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C75,$G75)), ($C75:$G75),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
@@ -6120,13 +6123,13 @@
       <c r="R76">
         <v>0</v>
       </c>
-      <c r="S76" t="e" cm="1">
+      <c r="S76" cm="1">
         <f t="array" aca="1" ref="S76" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C76,$G76)), ($C76:$G76),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T76" t="e" cm="1">
+        <v>282</v>
+      </c>
+      <c r="T76" cm="1">
         <f t="array" aca="1" ref="T76" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C76,$G76)), ($C76:$G76),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>358</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
@@ -6184,13 +6187,13 @@
       <c r="R77">
         <v>0</v>
       </c>
-      <c r="S77" t="e" cm="1">
+      <c r="S77" cm="1">
         <f t="array" aca="1" ref="S77" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C77,$G77)), ($C77:$G77),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T77" t="e" cm="1">
+        <v>72</v>
+      </c>
+      <c r="T77" cm="1">
         <f t="array" aca="1" ref="T77" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C77,$G77)), ($C77:$G77),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
@@ -6248,13 +6251,13 @@
       <c r="R78">
         <v>0</v>
       </c>
-      <c r="S78" t="e" cm="1">
+      <c r="S78" cm="1">
         <f t="array" aca="1" ref="S78" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C78,$G78)), ($C78:$G78),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T78" t="e" cm="1">
+        <v>51</v>
+      </c>
+      <c r="T78" cm="1">
         <f t="array" aca="1" ref="T78" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C78,$G78)), ($C78:$G78),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
@@ -6312,13 +6315,13 @@
       <c r="R79">
         <v>0</v>
       </c>
-      <c r="S79" t="e" cm="1">
+      <c r="S79" cm="1">
         <f t="array" aca="1" ref="S79" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C79,$G79)), ($C79:$G79),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T79" t="e" cm="1">
+        <v>54</v>
+      </c>
+      <c r="T79" cm="1">
         <f t="array" aca="1" ref="T79" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C79,$G79)), ($C79:$G79),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
@@ -6376,13 +6379,13 @@
       <c r="R80">
         <v>0</v>
       </c>
-      <c r="S80" t="e" cm="1">
+      <c r="S80" cm="1">
         <f t="array" aca="1" ref="S80" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C80,$G80)), ($C80:$G80),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T80" t="e" cm="1">
+        <v>123</v>
+      </c>
+      <c r="T80" cm="1">
         <f t="array" aca="1" ref="T80" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C80,$G80)), ($C80:$G80),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
@@ -6440,13 +6443,13 @@
       <c r="R81">
         <v>0</v>
       </c>
-      <c r="S81" t="e" cm="1">
+      <c r="S81" cm="1">
         <f t="array" aca="1" ref="S81" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C81,$G81)), ($C81:$G81),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T81" t="e" cm="1">
+        <v>345</v>
+      </c>
+      <c r="T81" cm="1">
         <f t="array" aca="1" ref="T81" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C81,$G81)), ($C81:$G81),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
@@ -6504,13 +6507,13 @@
       <c r="R82">
         <v>0</v>
       </c>
-      <c r="S82" t="e" cm="1">
+      <c r="S82" cm="1">
         <f t="array" aca="1" ref="S82" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C82,$G82)), ($C82:$G82),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T82" t="e" cm="1">
+        <v>27</v>
+      </c>
+      <c r="T82" cm="1">
         <f t="array" aca="1" ref="T82" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C82,$G82)), ($C82:$G82),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
@@ -6568,13 +6571,13 @@
       <c r="R83">
         <v>0</v>
       </c>
-      <c r="S83" t="e" cm="1">
+      <c r="S83" cm="1">
         <f t="array" aca="1" ref="S83" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C83,$G83)), ($C83:$G83),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T83" t="e" cm="1">
+        <v>387</v>
+      </c>
+      <c r="T83" cm="1">
         <f t="array" aca="1" ref="T83" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C83,$G83)), ($C83:$G83),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>542</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
@@ -6632,13 +6635,13 @@
       <c r="R84">
         <v>0</v>
       </c>
-      <c r="S84" t="e" cm="1">
+      <c r="S84" cm="1">
         <f t="array" aca="1" ref="S84" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C84,$G84)), ($C84:$G84),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T84" t="e" cm="1">
+        <v>2805</v>
+      </c>
+      <c r="T84" cm="1">
         <f t="array" aca="1" ref="T84" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C84,$G84)), ($C84:$G84),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
@@ -6696,13 +6699,13 @@
       <c r="R85">
         <v>0</v>
       </c>
-      <c r="S85" t="e" cm="1">
+      <c r="S85" cm="1">
         <f t="array" aca="1" ref="S85" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C85,$G85)), ($C85:$G85),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T85" t="e" cm="1">
+        <v>45</v>
+      </c>
+      <c r="T85" cm="1">
         <f t="array" aca="1" ref="T85" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C85,$G85)), ($C85:$G85),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
@@ -6760,13 +6763,13 @@
       <c r="R86">
         <v>0</v>
       </c>
-      <c r="S86" t="e" cm="1">
+      <c r="S86" cm="1">
         <f t="array" aca="1" ref="S86" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C86,$G86)), ($C86:$G86),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T86" t="e" cm="1">
+        <v>168</v>
+      </c>
+      <c r="T86" cm="1">
         <f t="array" aca="1" ref="T86" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C86,$G86)), ($C86:$G86),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
@@ -6824,13 +6827,13 @@
       <c r="R87">
         <v>0</v>
       </c>
-      <c r="S87" t="e" cm="1">
+      <c r="S87" cm="1">
         <f t="array" aca="1" ref="S87" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C87,$G87)), ($C87:$G87),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T87" t="e" cm="1">
+        <v>516</v>
+      </c>
+      <c r="T87" cm="1">
         <f t="array" aca="1" ref="T87" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C87,$G87)), ($C87:$G87),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>954</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
@@ -6888,13 +6891,13 @@
       <c r="R88">
         <v>0</v>
       </c>
-      <c r="S88" t="e" cm="1">
+      <c r="S88" cm="1">
         <f t="array" aca="1" ref="S88" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C88,$G88)), ($C88:$G88),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T88" t="e" cm="1">
+        <v>195</v>
+      </c>
+      <c r="T88" cm="1">
         <f t="array" aca="1" ref="T88" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C88,$G88)), ($C88:$G88),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
@@ -6952,13 +6955,13 @@
       <c r="R89">
         <v>0</v>
       </c>
-      <c r="S89" t="e" cm="1">
+      <c r="S89" cm="1">
         <f t="array" aca="1" ref="S89" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C89,$G89)), ($C89:$G89),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T89" t="e" cm="1">
+        <v>39</v>
+      </c>
+      <c r="T89" cm="1">
         <f t="array" aca="1" ref="T89" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C89,$G89)), ($C89:$G89),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
@@ -7016,13 +7019,13 @@
       <c r="R90">
         <v>0</v>
       </c>
-      <c r="S90" t="e" cm="1">
+      <c r="S90" cm="1">
         <f t="array" aca="1" ref="S90" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C90,$G90)), ($C90:$G90),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T90" t="e" cm="1">
+        <v>825</v>
+      </c>
+      <c r="T90" cm="1">
         <f t="array" aca="1" ref="T90" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C90,$G90)), ($C90:$G90),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
@@ -7080,13 +7083,13 @@
       <c r="R91">
         <v>0</v>
       </c>
-      <c r="S91" t="e" cm="1">
+      <c r="S91" cm="1">
         <f t="array" aca="1" ref="S91" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C91,$G91)), ($C91:$G91),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T91" t="e" cm="1">
+        <v>462</v>
+      </c>
+      <c r="T91" cm="1">
         <f t="array" aca="1" ref="T91" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C91,$G91)), ($C91:$G91),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>821</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
@@ -7144,13 +7147,13 @@
       <c r="R92">
         <v>0</v>
       </c>
-      <c r="S92" t="e" cm="1">
+      <c r="S92" cm="1">
         <f t="array" aca="1" ref="S92" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C92,$G92)), ($C92:$G92),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T92" t="e" cm="1">
+        <v>189</v>
+      </c>
+      <c r="T92" cm="1">
         <f t="array" aca="1" ref="T92" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C92,$G92)), ($C92:$G92),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
@@ -7205,13 +7208,13 @@
       <c r="R93">
         <v>5.48046875</v>
       </c>
-      <c r="S93" t="e" cm="1">
+      <c r="S93" cm="1">
         <f t="array" aca="1" ref="S93" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C93,$G93)), ($C93:$G93),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T93" t="e" cm="1">
+        <v>134</v>
+      </c>
+      <c r="T93" cm="1">
         <f t="array" aca="1" ref="T93" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C93,$G93)), ($C93:$G93),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
@@ -7266,13 +7269,13 @@
       <c r="R94">
         <v>0</v>
       </c>
-      <c r="S94" t="e" cm="1">
+      <c r="S94" cm="1">
         <f t="array" aca="1" ref="S94" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C94,$G94)), ($C94:$G94),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T94" t="e" cm="1">
+        <v>243</v>
+      </c>
+      <c r="T94" cm="1">
         <f t="array" aca="1" ref="T94" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C94,$G94)), ($C94:$G94),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
@@ -7327,13 +7330,13 @@
       <c r="R95">
         <v>0</v>
       </c>
-      <c r="S95" t="e" cm="1">
+      <c r="S95" cm="1">
         <f t="array" aca="1" ref="S95" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C95,$G95)), ($C95:$G95),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T95" t="e" cm="1">
+        <v>97</v>
+      </c>
+      <c r="T95" cm="1">
         <f t="array" aca="1" ref="T95" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C95,$G95)), ($C95:$G95),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
@@ -7388,13 +7391,13 @@
       <c r="R96">
         <v>12.482421875</v>
       </c>
-      <c r="S96" t="e" cm="1">
+      <c r="S96" cm="1">
         <f t="array" aca="1" ref="S96" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C96,$G96)), ($C96:$G96),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T96" t="e" cm="1">
+        <v>570</v>
+      </c>
+      <c r="T96" cm="1">
         <f t="array" aca="1" ref="T96" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C96,$G96)), ($C96:$G96),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>460</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
@@ -7449,13 +7452,13 @@
       <c r="R97">
         <v>0</v>
       </c>
-      <c r="S97" t="e" cm="1">
+      <c r="S97" cm="1">
         <f t="array" aca="1" ref="S97" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C97,$G97)), ($C97:$G97),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T97" t="e" cm="1">
+        <v>310</v>
+      </c>
+      <c r="T97" cm="1">
         <f t="array" aca="1" ref="T97" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C97,$G97)), ($C97:$G97),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>384</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
@@ -7510,13 +7513,13 @@
       <c r="R98">
         <v>13.5126953125</v>
       </c>
-      <c r="S98" t="e" cm="1">
+      <c r="S98" cm="1">
         <f t="array" aca="1" ref="S98" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C98,$G98)), ($C98:$G98),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T98" t="e" cm="1">
+        <v>570</v>
+      </c>
+      <c r="T98" cm="1">
         <f t="array" aca="1" ref="T98" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C98,$G98)), ($C98:$G98),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>674</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
@@ -7571,13 +7574,13 @@
       <c r="R99">
         <v>0</v>
       </c>
-      <c r="S99" t="e" cm="1">
+      <c r="S99" cm="1">
         <f t="array" aca="1" ref="S99" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C99,$G99)), ($C99:$G99),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T99" t="e" cm="1">
+        <v>162</v>
+      </c>
+      <c r="T99" cm="1">
         <f t="array" aca="1" ref="T99" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C99,$G99)), ($C99:$G99),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
@@ -7632,13 +7635,13 @@
       <c r="R100">
         <v>0</v>
       </c>
-      <c r="S100" t="e" cm="1">
+      <c r="S100" cm="1">
         <f t="array" aca="1" ref="S100" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C100,$G100)), ($C100:$G100),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T100" t="e" cm="1">
+        <v>46</v>
+      </c>
+      <c r="T100" cm="1">
         <f t="array" aca="1" ref="T100" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C100,$G100)), ($C100:$G100),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
@@ -7693,13 +7696,13 @@
       <c r="R101">
         <v>0</v>
       </c>
-      <c r="S101" t="e" cm="1">
+      <c r="S101" cm="1">
         <f t="array" aca="1" ref="S101" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C101,$G101)), ($C101:$G101),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T101" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="T101" cm="1">
         <f t="array" aca="1" ref="T101" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C101,$G101)), ($C101:$G101),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.2">
@@ -7754,13 +7757,13 @@
       <c r="R102">
         <v>0</v>
       </c>
-      <c r="S102" t="e" cm="1">
+      <c r="S102" cm="1">
         <f t="array" aca="1" ref="S102" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C102,$G102)), ($C102:$G102),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T102" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="T102" cm="1">
         <f t="array" aca="1" ref="T102" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C102,$G102)), ($C102:$G102),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>147</v>
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
@@ -7815,13 +7818,13 @@
       <c r="R103">
         <v>0</v>
       </c>
-      <c r="S103" t="e" cm="1">
+      <c r="S103" cm="1">
         <f t="array" aca="1" ref="S103" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C103,$G103)), ($C103:$G103),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T103" t="e" cm="1">
+        <v>94</v>
+      </c>
+      <c r="T103" cm="1">
         <f t="array" aca="1" ref="T103" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C103,$G103)), ($C103:$G103),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.2">
@@ -7876,13 +7879,13 @@
       <c r="R104">
         <v>0</v>
       </c>
-      <c r="S104" t="e" cm="1">
+      <c r="S104" cm="1">
         <f t="array" aca="1" ref="S104" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C104,$G104)), ($C104:$G104),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T104" t="e" cm="1">
+        <v>32</v>
+      </c>
+      <c r="T104" cm="1">
         <f t="array" aca="1" ref="T104" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C104,$G104)), ($C104:$G104),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
@@ -7937,13 +7940,34 @@
       <c r="R105">
         <v>32.6259765625</v>
       </c>
-      <c r="S105" t="e" cm="1">
+      <c r="S105" cm="1">
         <f t="array" aca="1" ref="S105" ca="1">INDIRECT(ADDRESS(ROW(), 2+_xlfn.XMATCH(MIN(($C105,$G105)), ($C105:$G105),0,1)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T105" t="e" cm="1">
+        <v>1136</v>
+      </c>
+      <c r="T105" cm="1">
         <f t="array" aca="1" ref="T105" ca="1">INDIRECT(ADDRESS(ROW(), 3+_xlfn.XMATCH(MIN(($C105,$G105)), ($C105:$G105),0,1)))</f>
-        <v>#VALUE!</v>
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106">
+        <f>GEOMEAN(C2:C105)</f>
+        <v>211.92269682687922</v>
+      </c>
+      <c r="G106">
+        <f>GEOMEAN(G2:G105)</f>
+        <v>209.96768833322389</v>
+      </c>
+      <c r="K106">
+        <f>GEOMEAN(K2:K105)</f>
+        <v>216.55289792072637</v>
+      </c>
+      <c r="S106">
+        <f ca="1">GEOMEAN(S2:S105)</f>
+        <v>203.24581308093201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>